<commit_message>
Commit README changes  - 24rd Sept
</commit_message>
<xml_diff>
--- a/src/steffs_pharmacy/data/invoices.xlsx
+++ b/src/steffs_pharmacy/data/invoices.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
@@ -928,6 +928,195 @@
         <v>15</v>
       </c>
     </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>SP24092022115848</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>101</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>PANADOL STRIP 20</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>3</v>
+      </c>
+      <c r="E24" t="n">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>SP24092022115848</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>100</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>PANADOL STRIP 10</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>6</v>
+      </c>
+      <c r="E25" t="n">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>SP24092022115848</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>109</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>ATORVASTATIN SANDOZ 10MG TABLETS 30</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>2</v>
+      </c>
+      <c r="E26" t="n">
+        <v>23.2</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>SP24092022120034</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>100</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>PANADOL STRIP 10</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>6</v>
+      </c>
+      <c r="E27" t="n">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>SP24092022120034</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>101</v>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>PANADOL STRIP 20</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>3</v>
+      </c>
+      <c r="E28" t="n">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>SP24092022120034</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>180</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>EPIDUO GEL 30g PUMP</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>2</v>
+      </c>
+      <c r="E29" t="n">
+        <v>110.76</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>SP24092022160310</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>100</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>PANADOL STRIP 10</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>4</v>
+      </c>
+      <c r="E30" t="n">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>SP24092022160310</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>102</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>NUROFEN STRIP 15</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>1</v>
+      </c>
+      <c r="E31" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>SP24092022160509</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>102</v>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>NUROFEN STRIP 15</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>1</v>
+      </c>
+      <c r="E32" t="n">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Commit MENU changes  - 25rd Sept
</commit_message>
<xml_diff>
--- a/src/steffs_pharmacy/data/invoices.xlsx
+++ b/src/steffs_pharmacy/data/invoices.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
@@ -1117,6 +1117,300 @@
         <v>12</v>
       </c>
     </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>SP25092022103921</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>100</v>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>PANADOL STRIP 10</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>2</v>
+      </c>
+      <c r="E33" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>SP25092022103921</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>103</v>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>NUROFEN STRIP 25</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>4</v>
+      </c>
+      <c r="E34" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>SP25092022104544</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>100</v>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>PANADOL STRIP 10</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>2</v>
+      </c>
+      <c r="E35" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>SP25092022104544</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>103</v>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>NUROFEN STRIP 25</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>2</v>
+      </c>
+      <c r="E36" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>SP25092022105145</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>100</v>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>PANADOL STRIP 10</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>5</v>
+      </c>
+      <c r="E37" t="n">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>SP25092022105145</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>103</v>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>NUROFEN STRIP 25</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>5</v>
+      </c>
+      <c r="E38" t="n">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>SP25092022105547</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>100</v>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>PANADOL STRIP 10</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>2</v>
+      </c>
+      <c r="E39" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>SP25092022105547</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>103</v>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>NUROFEN STRIP 25</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>4</v>
+      </c>
+      <c r="E40" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>SP25092022110035</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>100</v>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>PANADOL STRIP 10</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>2</v>
+      </c>
+      <c r="E41" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>SP25092022110035</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>103</v>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>NUROFEN STRIP 25</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>2</v>
+      </c>
+      <c r="E42" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>SP25092022110524</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>100</v>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>PANADOL STRIP 10</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>2</v>
+      </c>
+      <c r="E43" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>SP25092022110524</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>102</v>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>NUROFEN STRIP 15</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>2</v>
+      </c>
+      <c r="E44" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>SP25092022110937</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>100</v>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>PANADOL STRIP 10</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>2</v>
+      </c>
+      <c r="E45" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>SP25092022110937</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>102</v>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>NUROFEN STRIP 15</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>1</v>
+      </c>
+      <c r="E46" t="n">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Commit MENU case changes  - 25rd Sept
</commit_message>
<xml_diff>
--- a/src/steffs_pharmacy/data/invoices.xlsx
+++ b/src/steffs_pharmacy/data/invoices.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17340" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E46"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
@@ -1411,6 +1411,27 @@
         <v>12</v>
       </c>
     </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>SP25092022112318</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>100</v>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>PANADOL STRIP 10</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>1</v>
+      </c>
+      <c r="E47" t="n">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Commit shell script changes  - 25rd Sept
</commit_message>
<xml_diff>
--- a/src/steffs_pharmacy/data/invoices.xlsx
+++ b/src/steffs_pharmacy/data/invoices.xlsx
@@ -1,76 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steffy.johnson/projects/term1/python/pharmacy/src/steffs_pharmacy/data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{308C25A6-11EE-4347-80E2-C9C3788A9E7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17340" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
-  <si>
-    <t>INVOICE_NUMBER</t>
-  </si>
-  <si>
-    <t>MEDICINE_ID</t>
-  </si>
-  <si>
-    <t>MEDICINE_NAME</t>
-  </si>
-  <si>
-    <t>MEDICINE_QUANTITY</t>
-  </si>
-  <si>
-    <t>MEDICINE_PRICE</t>
-  </si>
-  <si>
-    <t>PANADOL STRIP 10</t>
-  </si>
-  <si>
-    <t>NUROFEN STRIP 15</t>
-  </si>
-  <si>
-    <t>SP25092022110937</t>
-  </si>
-  <si>
-    <t>SP25092022112318</t>
-  </si>
-  <si>
-    <t>SP25092022114003</t>
-  </si>
-  <si>
-    <t>SP25092022122137</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -89,21 +46,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -403,139 +419,219 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
+    <col width="17.33203125" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="12" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="17" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="19.1640625" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="15" bestFit="1" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>INVOICE_NUMBER</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>MEDICINE_ID</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>MEDICINE_NAME</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>MEDICINE_QUANTITY</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>MEDICINE_PRICE</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>SP25092022110937</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>100</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>PANADOL STRIP 10</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E2" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>SP25092022110937</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>102</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>NUROFEN STRIP 15</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E3" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>SP25092022112318</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>100</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>PANADOL STRIP 10</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>SP25092022114003</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>100</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>PANADOL STRIP 10</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E5" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>SP25092022114003</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>102</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>NUROFEN STRIP 15</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>SP25092022122137</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>100</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>PANADOL STRIP 10</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>7</v>
+      </c>
+      <c r="E7" t="n">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>SP25092022125102</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>100</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>PANADOL STRIP 10</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>2</v>
+      </c>
+      <c r="E8" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>SP25092022125102</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>102</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>NUROFEN STRIP 15</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2">
-        <v>100</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="E2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3">
-        <v>102</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4">
-        <v>100</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5">
-        <v>100</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6">
-        <v>102</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7">
-        <v>100</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7">
-        <v>7</v>
-      </c>
-      <c r="E7">
-        <v>105</v>
+      <c r="E9" t="n">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>